<commit_message>
rendmiento y redundancia Huffman
</commit_message>
<xml_diff>
--- a/TP2/Resultados/Datos-2daParte.xlsx
+++ b/TP2/Resultados/Datos-2daParte.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Ramiro\Documents\Facultad\3ro\2do Cuatri\Teoria de la Informacion\Repositorio\TP2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Ramiro\Documents\Facultad\3ro\2do Cuatri\Teoria de la Informacion\Repositorio\TP2\Resultados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEFD3125-2AE6-4F54-9885-0120098BC242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D360B155-1FAA-472A-9DAE-AB71D67569F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-210" yWindow="420" windowWidth="16380" windowHeight="15120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -113,7 +113,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,6 +131,14 @@
     </font>
     <font>
       <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -169,14 +177,14 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -461,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:F21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,10 +480,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
+      <c r="B1" s="6"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -484,12 +492,12 @@
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -558,7 +566,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="3">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
@@ -581,7 +589,7 @@
       </c>
       <c r="B8" s="3">
         <f>1-B5-B4-B6-B7</f>
-        <v>0</v>
+        <v>4.9999999999999989E-2</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>
@@ -631,19 +639,19 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="M15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="M15" s="4"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -660,7 +668,7 @@
       </c>
       <c r="B18">
         <f>B4*F5+B5*F6+B6*F7+B7*F8+B8*F9</f>
-        <v>0.35</v>
+        <v>0.33600000000000002</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -669,7 +677,7 @@
       </c>
       <c r="B19">
         <f>B4*G5+B5*G6+B6*G7+B7*G8+B8*G9</f>
-        <v>0.38599999999999995</v>
+        <v>0.39999999999999997</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -716,18 +724,18 @@
       </c>
       <c r="E23">
         <f>E8*B7/B17</f>
-        <v>0.34090909090909088</v>
+        <v>0.28409090909090906</v>
       </c>
       <c r="F23">
         <f>E9*B8/B17</f>
-        <v>0</v>
+        <v>5.6818181818181802E-2</v>
       </c>
       <c r="H23" t="s">
         <v>19</v>
       </c>
       <c r="I23">
-        <f>B23*LOG(1/B23,2) +C23*LOG(1/C23,2) + D23*LOG(1/D23,2) + E23*LOG(1/E23,2)</f>
-        <v>1.8588407364298161</v>
+        <f>B23*LOG(1/B23,2) +C23*LOG(1/C23,2) + D23*LOG(1/D23,2) + E23*LOG(1/E23,2)+F23*LOG(1/F23,2)</f>
+        <v>2.0804392892644823</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -736,30 +744,30 @@
       </c>
       <c r="B24">
         <f>F5*B4/$B$18</f>
-        <v>0.25714285714285717</v>
+        <v>0.26785714285714285</v>
       </c>
       <c r="C24">
         <f>F6*B5/$B$18</f>
-        <v>0.22857142857142862</v>
+        <v>0.23809523809523814</v>
       </c>
       <c r="D24">
         <f>B6*F7/$B$18</f>
-        <v>0.17142857142857143</v>
+        <v>0.17857142857142855</v>
       </c>
       <c r="E24">
         <f>B7*F8/$B$18</f>
-        <v>0.34285714285714286</v>
+        <v>0.29761904761904762</v>
       </c>
       <c r="F24">
         <f>B8*F9/$B$18</f>
-        <v>0</v>
+        <v>1.7857142857142853E-2</v>
       </c>
       <c r="H24" t="s">
         <v>20</v>
       </c>
       <c r="I24">
-        <f>B24*LOG(1/B24,2) +C24*LOG(1/C24,2) + D24*LOG(1/D24,2) + E24*LOG(1/E24,2)</f>
-        <v>1.9561787304889204</v>
+        <f>B24*LOG(1/B24,2) +C24*LOG(1/C24,2) + D24*LOG(1/D24,2) + E24*LOG(1/E24,2)+ F24*LOG(1/F24,2)</f>
+        <v>2.0699071371270636</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -768,30 +776,30 @@
       </c>
       <c r="B25">
         <f>G5*B4/$B$19</f>
-        <v>0.31088082901554404</v>
+        <v>0.3</v>
       </c>
       <c r="C25">
         <f>G6*B5/$B$19</f>
-        <v>0.24870466321243526</v>
+        <v>0.24000000000000002</v>
       </c>
       <c r="D25">
         <f>G7*B6/$B$19</f>
-        <v>0.20725388601036274</v>
+        <v>0.2</v>
       </c>
       <c r="E25">
         <f>G8*B7/$B$19</f>
-        <v>0.23316062176165803</v>
+        <v>0.18749999999999997</v>
       </c>
       <c r="F25">
         <f>B8*G9/$B$19</f>
-        <v>0</v>
+        <v>7.2499999999999981E-2</v>
       </c>
       <c r="H25" t="s">
         <v>21</v>
       </c>
       <c r="I25">
-        <f>B25*LOG(1/B25,2) +C25*LOG(1/C25,2) + D25*LOG(1/D25,2) + E25*LOG(1/E25,2)</f>
-        <v>1.9836376129082025</v>
+        <f>B25*LOG(1/B25,2) +C25*LOG(1/C25,2) + D25*LOG(1/D25,2) + E25*LOG(1/E25,2)+F25*LOG(1/F25,2)</f>
+        <v>2.2069052653268924</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -800,7 +808,7 @@
       </c>
       <c r="I27">
         <f>B17*I23+B18*I24+B19*I25</f>
-        <v>1.9410806286711599</v>
+        <v>2.1274868765712736</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -808,8 +816,8 @@
         <v>23</v>
       </c>
       <c r="I29">
-        <f>B4*LOG(1/B4,2)+B5*LOG(1/B5,2)+B6*LOG(1/B6,2)+B7*LOG(1/B7,2)</f>
-        <v>1.9709505944546688</v>
+        <f>B4*LOG(1/B4,2)+B5*LOG(1/B5,2)+B6*LOG(1/B6,2)+B7*LOG(1/B7,2)+B8*LOG(1/B8,2)</f>
+        <v>2.1659573209491749</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -818,7 +826,7 @@
       </c>
       <c r="I31">
         <f>I29-I27</f>
-        <v>2.9869965783508867E-2</v>
+        <v>3.8470444377901369E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>